<commit_message>
adición de evidencias de aprendizaje de Marisol
</commit_message>
<xml_diff>
--- a/algebra.xlsx
+++ b/algebra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\1_algebra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2FFE1316-ADA3-49CE-AFF6-4BA991BFD2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2C149D-04EF-42BE-BC90-354DF6300F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="algebra" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Nombre</t>
   </si>
@@ -200,12 +200,15 @@
   </si>
   <si>
     <t>tejadavanesa7@gmail.com</t>
+  </si>
+  <si>
+    <t>q1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -683,8 +686,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1039,11 +1045,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1052,23 +1058,29 @@
     <col min="2" max="2" width="40.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1076,7 +1088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1084,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1092,7 +1104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1100,7 +1112,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1108,7 +1120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1116,7 +1128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1124,7 +1136,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1132,7 +1144,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1140,7 +1152,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1148,7 +1160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1156,7 +1168,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1164,7 +1176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1172,7 +1184,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>

</xml_diff>